<commit_message>
Added log File and Extent reports
</commit_message>
<xml_diff>
--- a/src/main/DataFromExcel/TaskData.xlsx
+++ b/src/main/DataFromExcel/TaskData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuchander\Api_testing_maven\src\main\DataFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD066B21-543F-44E4-BDBB-123646B8391D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F769056C-3DFF-4C52-B43B-D2B132F4AB62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,9 +372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -476,6 +478,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>12345</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
resloved adding 20 tasks at a time issue
</commit_message>
<xml_diff>
--- a/src/main/DataFromExcel/TaskData.xlsx
+++ b/src/main/DataFromExcel/TaskData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vuchander\Api_testing_maven\src\main\DataFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F769056C-3DFF-4C52-B43B-D2B132F4AB62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94FF797-B477-4D20-9BDA-8C3E710B70DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Reading book</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>gym</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,8 +482,13 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>12345</v>
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>